<commit_message>
docs(Investimentos): ORB-1077 - Ajustar planilha, excel e deixar um espaço entre a imagem e o texto.
</commit_message>
<xml_diff>
--- a/documentation/source/images/extras/tabela_api_investimentos_classificacao_denominacao.xlsx
+++ b/documentation/source/images/extras/tabela_api_investimentos_classificacao_denominacao.xlsx
@@ -17,6 +17,13 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Classificação no atributo </t>
     </r>
     <r>
@@ -38,7 +45,7 @@
     <t>2. Ações</t>
   </si>
   <si>
-    <t>3. Fundo de ìndices</t>
+    <t>3. Fundo de índices</t>
   </si>
   <si>
     <t>4. Tesouro Direto</t>
@@ -151,10 +158,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -196,6 +203,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -203,22 +232,84 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,108 +323,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,13 +381,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,169 +519,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,8 +692,47 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,17 +752,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,197 +786,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,10 +1296,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E21"/>
+  <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -1301,6 +1308,7 @@
     <col min="2" max="5" width="43.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.5"/>
     <row r="2" ht="16.5" spans="2:5">
       <c r="B2" s="1" t="s">
         <v>0</v>

</xml_diff>